<commit_message>
Adding the RestAssuredFW project
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/api/gorest/testdata/GorestTestData.xlsx
+++ b/src/main/java/com/qa/api/gorest/testdata/GorestTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E0F6D594-ED97-4266-AFD2-CBB345675B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D38B7502-F117-41F9-99EA-F515E1C58B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="19460" windowHeight="11060" xr2:uid="{8DC102DE-BB99-4EC9-BB1B-30E319DD645A}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>abu1@gmail.com</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -50,25 +47,28 @@
     <t>Female</t>
   </si>
   <si>
-    <t>pallu1@gmail.com</t>
-  </si>
-  <si>
-    <t>zarina1@gmail.com</t>
-  </si>
-  <si>
-    <t>tahira1@gmail.com</t>
-  </si>
-  <si>
-    <t>Abu3</t>
-  </si>
-  <si>
-    <t>Pallu3</t>
-  </si>
-  <si>
-    <t>Zarina3</t>
-  </si>
-  <si>
-    <t>Tahira3</t>
+    <t>Abu4</t>
+  </si>
+  <si>
+    <t>Pallu4</t>
+  </si>
+  <si>
+    <t>Zarina4</t>
+  </si>
+  <si>
+    <t>Tahira4</t>
+  </si>
+  <si>
+    <t>abu4@gmail.com</t>
+  </si>
+  <si>
+    <t>pallu4@gmail.com</t>
+  </si>
+  <si>
+    <t>zarina4@gmail.com</t>
+  </si>
+  <si>
+    <t>tahira4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,58 +461,58 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing the data in the GorestTestData.xlsx
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/api/gorest/testdata/GorestTestData.xlsx
+++ b/src/main/java/com/qa/api/gorest/testdata/GorestTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D38B7502-F117-41F9-99EA-F515E1C58B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{581977F2-B81D-4A7C-99AC-4211C5A19633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19460" windowHeight="11060" xr2:uid="{8DC102DE-BB99-4EC9-BB1B-30E319DD645A}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19460" windowHeight="11060" xr2:uid="{8DC102DE-BB99-4EC9-BB1B-30E319DD645A}"/>
   </bookViews>
   <sheets>
     <sheet name="userdata" sheetId="1" r:id="rId1"/>
@@ -59,16 +59,16 @@
     <t>Tahira4</t>
   </si>
   <si>
-    <t>abu4@gmail.com</t>
-  </si>
-  <si>
-    <t>pallu4@gmail.com</t>
-  </si>
-  <si>
-    <t>zarina4@gmail.com</t>
-  </si>
-  <si>
-    <t>tahira4@gmail.com</t>
+    <t>abu10@gmail.com</t>
+  </si>
+  <si>
+    <t>pallu10@gmail.com</t>
+  </si>
+  <si>
+    <t>zarina10@gmail.com</t>
+  </si>
+  <si>
+    <t>tahira10@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>